<commit_message>
Achieves convergence for the time-stepping S2FEM!
</commit_message>
<xml_diff>
--- a/tests/icosahedron-l2e.xlsx
+++ b/tests/icosahedron-l2e.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\cartosphere\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C27D6-C544-4F6F-A72F-24B2C5136179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6376ABC-4CE5-4C59-B095-A198ED6B0239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{03127F11-0492-4042-A9DA-79E4682E0194}"/>
+    <workbookView xWindow="7935" yWindow="4980" windowWidth="18255" windowHeight="8985" activeTab="2" xr2:uid="{03127F11-0492-4042-A9DA-79E4682E0194}"/>
   </bookViews>
   <sheets>
-    <sheet name="Case 1" sheetId="1" r:id="rId1"/>
+    <sheet name="res c 1 0" sheetId="2" r:id="rId1"/>
+    <sheet name="res a scenario 0" sheetId="1" r:id="rId2"/>
+    <sheet name="res a scenario 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>File:</t>
   </si>
@@ -66,6 +68,21 @@
   </si>
   <si>
     <t>Steady-state</t>
+  </si>
+  <si>
+    <t>Y_1^0</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2Y_1^0</t>
+  </si>
+  <si>
+    <t>x^2+y^2-2/3</t>
+  </si>
+  <si>
+    <t>-lapl u</t>
   </si>
 </sst>
 </file>
@@ -101,12 +118,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -181,7 +202,393 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Case 1'!$C$3</c:f>
+              <c:f>'res c 1 0'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L2-error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'res c 1 0'!$B$4:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3047200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72972800000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37742100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19040599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5419000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.77367E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3871699999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'res c 1 0'!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.2191100000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9832199999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4819099999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1953599999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.54864E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>3.8719900000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>9.7864300000000004E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D8F-4F01-AE41-A6E3813D6778}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="361205088"/>
+        <c:axId val="358580096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="361205088"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358580096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358580096"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361205088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'res a scenario 0'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -264,7 +671,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Case 1'!$B$4:$B$10</c:f>
+              <c:f>'res a scenario 0'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -294,7 +701,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Case 1'!$C$4:$C$10</c:f>
+              <c:f>'res a scenario 0'!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -518,7 +925,473 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'res a scenario 1'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L2-error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'res a scenario 1'!$B$4:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3047200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72972800000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37742100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19040599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5419000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.77367E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3871699999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'res a scenario 1'!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.40706999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.113691</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9236499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3719399999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.84771E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>4.6227900000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>1.1559499999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-37CC-494B-98E6-F3C51CE0C777}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="361205088"/>
+        <c:axId val="358580096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="361205088"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358580096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358580096"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361205088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1074,7 +1947,1080 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8591177-010D-48CC-880F-6183AF3F92F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1099,6 +3045,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF474AD-4403-4B68-8B08-826228FCE9F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1411,18 +3400,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB97A9D-38C3-442A-9322-C76F175F6339}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8B47C4-F674-4217-8B06-ED489CD90B8A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,7 +3449,7 @@
         <v>1.3047200000000001</v>
       </c>
       <c r="C4">
-        <v>1.3048500000000001</v>
+        <v>4.2191100000000002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +3460,7 @@
         <v>0.72972800000000004</v>
       </c>
       <c r="C5">
-        <v>0.301589</v>
+        <v>9.9832199999999992E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,7 +3471,7 @@
         <v>0.37742100000000001</v>
       </c>
       <c r="C6">
-        <v>7.6234099999999999E-2</v>
+        <v>2.4819099999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1493,7 +3482,7 @@
         <v>0.19040599999999999</v>
       </c>
       <c r="C7">
-        <v>1.9292199999999999E-2</v>
+        <v>6.1953599999999996E-4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1504,7 +3493,7 @@
         <v>9.5419000000000004E-2</v>
       </c>
       <c r="C8">
-        <v>4.8504799999999999E-3</v>
+        <v>1.54864E-4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1514,8 +3503,8 @@
       <c r="B9">
         <v>4.77367E-2</v>
       </c>
-      <c r="C9">
-        <v>1.2151499999999999E-3</v>
+      <c r="C9" s="3">
+        <v>3.8719900000000002E-5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,36 +3514,341 @@
       <c r="B10">
         <v>2.3871699999999999E-2</v>
       </c>
-      <c r="C10">
-        <v>3.0399700000000002E-4</v>
-      </c>
+      <c r="C10" s="3">
+        <v>9.7864300000000004E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2">
-        <v>0</v>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
-        <v>2</v>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB97A9D-38C3-442A-9322-C76F175F6339}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.3047200000000001</v>
+      </c>
+      <c r="C4">
+        <v>1.3048500000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.72972800000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.301589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.37742100000000001</v>
+      </c>
+      <c r="C6">
+        <v>7.6234099999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.19040599999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.9292199999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>9.5419000000000004E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.8504799999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>4.77367E-2</v>
+      </c>
+      <c r="C9">
+        <v>1.2151499999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>2.3871699999999999E-2</v>
+      </c>
+      <c r="C10">
+        <v>3.0399700000000002E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0C200E-6242-4416-B08E-1746CC2DCC88}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.3047200000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.40706999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.72972800000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.113691</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.37742100000000001</v>
+      </c>
+      <c r="C6">
+        <v>2.9236499999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.19040599999999999</v>
+      </c>
+      <c r="C7">
+        <v>7.3719399999999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>9.5419000000000004E-2</v>
+      </c>
+      <c r="C8">
+        <v>1.84771E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>4.77367E-2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.6227900000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>2.3871699999999999E-2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.1559499999999999E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>